<commit_message>
Final commit with README
</commit_message>
<xml_diff>
--- a/Results/Final Results/Scenarios/Scenarios_03_Format.xlsx
+++ b/Results/Final Results/Scenarios/Scenarios_03_Format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\6.Semester\Bachelor-Arbeit\bachelor-thesis\bachelor-thesis\Results\Final Results\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F6074B-B71E-4D32-885F-6E77F5A375FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B373A5-F42C-4D3A-8504-B708ADA5E330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,12 +174,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -191,6 +191,9 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -268,9 +271,6 @@
       </font>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -317,14 +317,14 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" uniqueName="2" name="Tolerance Ɛ" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" uniqueName="3" name="Step Size Rule" queryTableFieldId="3"/>
     <tableColumn id="15" xr3:uid="{A4350A9B-BCC6-44F5-A116-85913DA7D665}" uniqueName="15" name="Naïve" queryTableFieldId="8"/>
-    <tableColumn id="16" xr3:uid="{6B9F47BC-1FCA-4195-89B9-2044F5ED292F}" uniqueName="16" name="(Gap Naïve)" queryTableFieldId="7" dataDxfId="3" dataCellStyle="Prozent"/>
-    <tableColumn id="17" xr3:uid="{91E704B1-85F4-4A80-9B3B-3312315BB7CE}" uniqueName="17" name="LR" queryTableFieldId="9" dataDxfId="2" dataCellStyle="Prozent"/>
-    <tableColumn id="18" xr3:uid="{D575BB26-41C7-4859-B063-93806495F978}" uniqueName="18" name="(Gap LR)" queryTableFieldId="6" dataDxfId="1" dataCellStyle="Prozent"/>
-    <tableColumn id="19" xr3:uid="{7BBDAA48-9D88-43C9-92B5-D1FBE41553D7}" uniqueName="19" name="Naive" queryTableFieldId="11" dataDxfId="0" dataCellStyle="Prozent"/>
+    <tableColumn id="16" xr3:uid="{6B9F47BC-1FCA-4195-89B9-2044F5ED292F}" uniqueName="16" name="(Gap Naïve)" queryTableFieldId="7" dataDxfId="4" dataCellStyle="Prozent"/>
+    <tableColumn id="17" xr3:uid="{91E704B1-85F4-4A80-9B3B-3312315BB7CE}" uniqueName="17" name="LR" queryTableFieldId="9" dataDxfId="3" dataCellStyle="Prozent"/>
+    <tableColumn id="18" xr3:uid="{D575BB26-41C7-4859-B063-93806495F978}" uniqueName="18" name="(Gap LR)" queryTableFieldId="6" dataDxfId="2" dataCellStyle="Prozent"/>
+    <tableColumn id="19" xr3:uid="{7BBDAA48-9D88-43C9-92B5-D1FBE41553D7}" uniqueName="19" name="Naive" queryTableFieldId="11" dataDxfId="1" dataCellStyle="Prozent"/>
     <tableColumn id="22" xr3:uid="{4BA4B43F-2746-4D59-878A-FA4C3F29B4B1}" uniqueName="22" name="L R" queryTableFieldId="22"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" uniqueName="4" name="Iterations" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" uniqueName="5" name="Convergence" queryTableFieldId="5"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" uniqueName="10" name="Gap" queryTableFieldId="10" dataDxfId="4" dataCellStyle="Prozent"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" uniqueName="10" name="Gap" queryTableFieldId="10" dataDxfId="0" dataCellStyle="Prozent"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -630,7 +630,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,7 +642,7 @@
     <col min="5" max="5" width="15.36328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.81640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.90625" customWidth="1"/>
@@ -650,29 +650,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
       <c r="H1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="5"/>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -693,7 +693,7 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
@@ -731,7 +731,7 @@
       <c r="G3" s="1">
         <v>2.3400000000000001E-3</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>107</v>
       </c>
       <c r="I3">
@@ -769,7 +769,7 @@
       <c r="G4" s="1">
         <v>3.4099999999999998E-3</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>107</v>
       </c>
       <c r="I4">
@@ -807,7 +807,7 @@
       <c r="G5" s="1">
         <v>2.8700000000000002E-3</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>107</v>
       </c>
       <c r="I5">
@@ -845,7 +845,7 @@
       <c r="G6" s="1">
         <v>3.0799999999999998E-3</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>107</v>
       </c>
       <c r="I6">
@@ -883,7 +883,7 @@
       <c r="G7" s="1">
         <v>3.4099999999999998E-3</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>107</v>
       </c>
       <c r="I7">
@@ -921,7 +921,7 @@
       <c r="G8" s="1">
         <v>2.31E-3</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>107</v>
       </c>
       <c r="I8">
@@ -959,7 +959,7 @@
       <c r="G9" s="1">
         <v>2.1950000000000001E-2</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>641</v>
       </c>
       <c r="I9">
@@ -997,7 +997,7 @@
       <c r="G10" s="1">
         <v>2.1950000000000001E-2</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>641</v>
       </c>
       <c r="I10">
@@ -1035,7 +1035,7 @@
       <c r="G11" s="1">
         <v>2.1950000000000001E-2</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>641</v>
       </c>
       <c r="I11">
@@ -1073,7 +1073,7 @@
       <c r="G12" s="1">
         <v>2.1950000000000001E-2</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>641</v>
       </c>
       <c r="I12">
@@ -1111,7 +1111,7 @@
       <c r="G13" s="1">
         <v>2.1950000000000001E-2</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>641</v>
       </c>
       <c r="I13">
@@ -1149,7 +1149,7 @@
       <c r="G14" s="1">
         <v>2.1950000000000001E-2</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>641</v>
       </c>
       <c r="I14">
@@ -1187,7 +1187,7 @@
       <c r="G15" s="1">
         <v>2.9680000000000002E-2</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>2937</v>
       </c>
       <c r="I15">
@@ -1225,7 +1225,7 @@
       <c r="G16" s="1">
         <v>2.9680000000000002E-2</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <v>2937</v>
       </c>
       <c r="I16">
@@ -1263,7 +1263,7 @@
       <c r="G17" s="1">
         <v>2.9680000000000002E-2</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>2937</v>
       </c>
       <c r="I17">
@@ -1301,7 +1301,7 @@
       <c r="G18" s="1">
         <v>2.9680000000000002E-2</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <v>2937</v>
       </c>
       <c r="I18">
@@ -1339,7 +1339,7 @@
       <c r="G19" s="1">
         <v>2.9680000000000002E-2</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <v>2937</v>
       </c>
       <c r="I19">
@@ -1377,7 +1377,7 @@
       <c r="G20" s="1">
         <v>2.9010000000000001E-2</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <v>2937</v>
       </c>
       <c r="I20">
@@ -1415,7 +1415,7 @@
       <c r="G21" s="1">
         <v>2.971E-2</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <v>1889</v>
       </c>
       <c r="I21">
@@ -1453,7 +1453,7 @@
       <c r="G22" s="1">
         <v>2.971E-2</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <v>1889</v>
       </c>
       <c r="I22">
@@ -1491,7 +1491,7 @@
       <c r="G23" s="1">
         <v>2.971E-2</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <v>1889</v>
       </c>
       <c r="I23">
@@ -1529,7 +1529,7 @@
       <c r="G24" s="1">
         <v>2.971E-2</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="3">
         <v>1889</v>
       </c>
       <c r="I24">
@@ -1567,7 +1567,7 @@
       <c r="G25" s="1">
         <v>2.971E-2</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="3">
         <v>1889</v>
       </c>
       <c r="I25">
@@ -1605,7 +1605,7 @@
       <c r="G26" s="1">
         <v>2.971E-2</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="3">
         <v>1889</v>
       </c>
       <c r="I26">
@@ -1643,7 +1643,7 @@
       <c r="G27" s="1">
         <v>2.1569999999999999E-2</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <v>3527</v>
       </c>
       <c r="I27">
@@ -1681,7 +1681,7 @@
       <c r="G28" s="1">
         <v>2.1770000000000001E-2</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="3">
         <v>3527</v>
       </c>
       <c r="I28">
@@ -1719,7 +1719,7 @@
       <c r="G29" s="1">
         <v>2.1770000000000001E-2</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="3">
         <v>3527</v>
       </c>
       <c r="I29">
@@ -1757,7 +1757,7 @@
       <c r="G30" s="1">
         <v>2.1770000000000001E-2</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="3">
         <v>3527</v>
       </c>
       <c r="I30">
@@ -1795,7 +1795,7 @@
       <c r="G31" s="1">
         <v>2.196E-2</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="3">
         <v>3527</v>
       </c>
       <c r="I31">
@@ -1833,7 +1833,7 @@
       <c r="G32" s="1">
         <v>2.196E-2</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32" s="3">
         <v>3527</v>
       </c>
       <c r="I32">
@@ -1871,7 +1871,7 @@
       <c r="G33" s="1">
         <v>0</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="3">
         <v>4244</v>
       </c>
       <c r="I33">
@@ -1909,7 +1909,7 @@
       <c r="G34" s="1">
         <v>0</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="3">
         <v>4244</v>
       </c>
       <c r="I34">
@@ -1947,7 +1947,7 @@
       <c r="G35" s="1">
         <v>0</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="3">
         <v>4244</v>
       </c>
       <c r="I35">
@@ -1985,7 +1985,7 @@
       <c r="G36" s="1">
         <v>2.094E-2</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <v>4244</v>
       </c>
       <c r="I36">
@@ -2023,7 +2023,7 @@
       <c r="G37" s="1">
         <v>2.9010000000000001E-2</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <v>4244</v>
       </c>
       <c r="I37">
@@ -2061,7 +2061,7 @@
       <c r="G38" s="1">
         <v>3.4770000000000002E-2</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <v>4244</v>
       </c>
       <c r="I38">

</xml_diff>